<commit_message>
Update 9/29 - many many changes
</commit_message>
<xml_diff>
--- a/BODY nodes.xlsx
+++ b/BODY nodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b18041e678fb695/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec Helm\Daughters_of_the_Wreath-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{A83B68CE-6F46-42B8-A4A0-27C0313FD1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CEB625-9064-4E0D-B850-92C92B7F922B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7887409-3A47-459F-B2E2-B0BB13CE1AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE1BD494-E09C-4F03-B2FE-71837A6921F2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE1BD494-E09C-4F03-B2FE-71837A6921F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
-  <si>
-    <t>Node Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>HP</t>
   </si>
@@ -50,15 +47,6 @@
     <t>Durability</t>
   </si>
   <si>
-    <t>Fast Regen</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Damage</t>
-  </si>
-  <si>
     <t>Strength</t>
   </si>
   <si>
@@ -77,18 +65,12 @@
     <t>Piercing Precision</t>
   </si>
   <si>
-    <t>Bludgeoning precision</t>
-  </si>
-  <si>
     <t>Ranged Precision</t>
   </si>
   <si>
     <t>Thrown Precision</t>
   </si>
   <si>
-    <t>Shields Precision</t>
-  </si>
-  <si>
     <t>Parrying Precision</t>
   </si>
   <si>
@@ -182,7 +164,163 @@
     <t>Wreath Wrecker</t>
   </si>
   <si>
-    <t>Athletic Mastery</t>
+    <t>Node ID</t>
+  </si>
+  <si>
+    <t>Increases HP by 2</t>
+  </si>
+  <si>
+    <t>Increases Slow Regen by 1</t>
+  </si>
+  <si>
+    <t>Increases Heavy Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Standard Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Light Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Ranged Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Shield Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Slashing Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Piercing Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Bludgeoning Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Thrown Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Parrying Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Normal Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Great Precision by 1</t>
+  </si>
+  <si>
+    <t>Increases Heavy Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Standard Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Light Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Ranged Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Slashing Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Piercing Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Bludgeoning Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Thrown Damage by 1</t>
+  </si>
+  <si>
+    <t>Increases Durability by 1</t>
+  </si>
+  <si>
+    <t>Increases Strength by 1</t>
+  </si>
+  <si>
+    <t>Written Description</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>["HP"] += 2</t>
+  </si>
+  <si>
+    <t>["Slow Regen"] += 1</t>
+  </si>
+  <si>
+    <t>["Durability"] += 1</t>
+  </si>
+  <si>
+    <t>["Heavy Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Standard Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Light Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Ranged Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Shield Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Slashing Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Piercing Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Bludgeoning Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Thrown Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Parrying Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Normal Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Great Precision"] += 1</t>
+  </si>
+  <si>
+    <t>["Strength"] += 1</t>
+  </si>
+  <si>
+    <t>["Heavy Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Standard Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Light Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Ranged Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Slashing Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Piercing Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Bludgeoning Damage"] += 1</t>
+  </si>
+  <si>
+    <t>["Thrown Damage"] += 1</t>
+  </si>
+  <si>
+    <t>Athletics Mastery</t>
+  </si>
+  <si>
+    <t>Health Mastery</t>
   </si>
 </sst>
 </file>
@@ -543,414 +681,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729F6733-FE3B-4132-874C-A879F3F5C577}">
-  <dimension ref="A1:AB45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="W20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>